<commit_message>
Aggiunta la gestione del file di bow
</commit_message>
<xml_diff>
--- a/Files/template.xlsx
+++ b/Files/template.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24120" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="24120" windowHeight="12915" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Algoritmo" sheetId="1" r:id="rId1"/>
     <sheet name="Emoticons" sheetId="2" r:id="rId2"/>
-    <sheet name="Grafici" sheetId="3" r:id="rId3"/>
+    <sheet name="Bow" sheetId="4" r:id="rId3"/>
+    <sheet name="Grafici" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="output" localSheetId="0">Algoritmo!$A$2:$E$289</definedName>
@@ -259,11 +260,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163709312"/>
-        <c:axId val="163710848"/>
+        <c:axId val="156180864"/>
+        <c:axId val="156182400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163709312"/>
+        <c:axId val="156180864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -273,7 +274,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163710848"/>
+        <c:crossAx val="156182400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -281,7 +282,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163710848"/>
+        <c:axId val="156182400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -292,14 +293,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163709312"/>
+        <c:crossAx val="156180864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -460,11 +460,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="163758080"/>
-        <c:axId val="163759616"/>
+        <c:axId val="156225536"/>
+        <c:axId val="156227072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="163758080"/>
+        <c:axId val="156225536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,7 +474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163759616"/>
+        <c:crossAx val="156227072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -482,7 +482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="163759616"/>
+        <c:axId val="156227072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -493,7 +493,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163758080"/>
+        <c:crossAx val="156225536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -594,11 +594,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="168650624"/>
-        <c:axId val="168652160"/>
+        <c:axId val="157251456"/>
+        <c:axId val="157252992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="168650624"/>
+        <c:axId val="157251456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -608,7 +608,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168652160"/>
+        <c:crossAx val="157252992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -616,7 +616,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168652160"/>
+        <c:axId val="157252992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -627,7 +627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168650624"/>
+        <c:crossAx val="157251456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1087,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F289"/>
     </sheetView>
   </sheetViews>
@@ -1130,6 +1130,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>

</xml_diff>